<commit_message>
Adds meta data import for havo
</commit_message>
<xml_diff>
--- a/vwoa.xlsx
+++ b/vwoa.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bertjan/Projects/examenfit/api/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFBECEFE-4257-2341-942C-4ACAD763F4DD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93DC2579-CA8C-3242-A8EB-E3934138F942}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33480" windowHeight="37800" xr2:uid="{6DFEB707-863B-7B40-8FCC-4842B800C519}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33480" windowHeight="37300" xr2:uid="{6DFEB707-863B-7B40-8FCC-4842B800C519}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Blad1!$A$1:$R$1</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1868,13 +1868,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{749BD3E2-6636-194F-BBA3-EAD7A6486513}">
   <dimension ref="A1:R139"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+    <sheetView tabSelected="1" topLeftCell="A107" workbookViewId="0">
+      <selection activeCell="A133" sqref="A133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="37.83203125" customWidth="1"/>
     <col min="3" max="3" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="43.33203125" customWidth="1"/>
+    <col min="5" max="5" width="34.83203125" customWidth="1"/>
     <col min="7" max="7" width="12.83203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17.1640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="33" bestFit="1" customWidth="1"/>
@@ -8572,5 +8575,6 @@
   </sheetData>
   <autoFilter ref="A1:R1" xr:uid="{187DD16F-A7F9-1C49-AFBC-B13EF475C825}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>